<commit_message>
Added basic Event listeners, Log4j2 logs. To be implemented extensively in future
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/oneWayFlight_checkEconomyClassResultsDefaultDate.xlsx
+++ b/src/test/resources/testData/oneWayFlight_checkEconomyClassResultsDefaultDate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\WebTesting\WebTesting\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A100BA3-BD3F-4474-9A31-F2B2CF86D05B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AB4C0F-0072-40AD-8505-327223877D9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>1</v>

</xml_diff>